<commit_message>
Filter Applied for Product Year
Filter Applied for Product announced year in socialmediascraping.html
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Product</t>
   </si>
@@ -29,26 +29,17 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Sony Xperia XZ3</t>
-  </si>
-  <si>
-    <t>02/18/2019</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/sony_xperia_xz3-reviews-9232p1.php</t>
-  </si>
-  <si>
-    <t>Anonymous, 18 Feb 2019Wrong, Casio released the first waterproof phone. Sony copied.u meant World 1st waterproof SMARTPHONE (Sony Xperia Z) Not A  Obama phone  LuL ..!</t>
-  </si>
-  <si>
-    <t>Anonymous, 16 Feb 2019Sony is the first to launch waterproof and dust resistant phone way back 2011. 3.5 jack and so... moreWrong, Casio released the first waterproof phone. Sony copied.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bai suzhen, 17 Feb 2019 Nope. The code is open.  All people in the world can read it.
-So all brands now have the sam... morewoohooo foldable  phones so amazing </t>
-  </si>
-  <si>
-    <t>Hdh, 17 Feb 2019Too thick and long!!!!!!!! Remove the sony logo! Improve battery life!! Ill buy one. It already has higher battery endurance than most other flagships on the market. After using it for the past 4 months, I can say it doesn't feel thick at all. It's definitely a bit heavier than other phones the same size, but that's a sign of sturdy build quality. There's plenty of tempered glass protectors out there that will also cover up the logo for you. I'm actually using one.</t>
+    <t>Apple iPhone XS Max</t>
+  </si>
+  <si>
+    <t>02/20/2019</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/apple_iphone_xs_max-reviews-9319p1.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I just love using this phone
+</t>
   </si>
 </sst>
 </file>
@@ -397,7 +388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,48 +424,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
changes in gsmarena get issue
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Product</t>
   </si>
@@ -29,39 +28,111 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Apple iPhone XS Max</t>
-  </si>
-  <si>
-    <t>02/20/2019</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/apple_iphone_xs_max-reviews-9319p1.php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I just love using this phone
+    <t>Samsung Galaxy S10 5G</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/samsung_galaxy_s10_5g-reviews-9588.php</t>
+  </si>
+  <si>
+    <t>Looks sucks 3 camera setup on front</t>
+  </si>
+  <si>
+    <t>as long as the battery not exploding, it's good device.</t>
+  </si>
+  <si>
+    <t>Not bad idea for investment, cause it's already capable 5G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With regards to European customers : does the Exynos 9820 Octa (8 nm) - EMEA actually offer 5G ? I thought only the Qualcomm Snapdragon 855 (USA/LATAM, China) offer 5G ?
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very big screen and big in size </t>
+  </si>
+  <si>
+    <t>Samsung didnt meet my expectations at all. highly disappointed.</t>
+  </si>
+  <si>
+    <t>insanely big phone,no card slot.What a waste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anonymous, 15 hours agoNot a good size for a phone . It should be little bigger then this because it's a tablet   . L... moreDont be stupidd. Mi max 4 hasn't release yet. </t>
+  </si>
+  <si>
+    <t>Dead pixel on screen? niceee</t>
+  </si>
+  <si>
+    <t>New display technology?</t>
+  </si>
+  <si>
+    <t>The only highlight is the 5G and the S10+ is the 1TB Internal Storage, wish they combine those two features into one, too many options.</t>
+  </si>
+  <si>
+    <t>Not a good</t>
+  </si>
+  <si>
+    <t>Better looking with a normal center notch than this black ugly bar in display..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Natan, 14 hours agoAgreed. I'm excited to see what Huawei brings with the P30.camera huawei mach mach better...battery stronger...sorry but Samsung battery life ans camera low level.... _x000D_
+still huawei on positive place ....
+</t>
+  </si>
+  <si>
+    <t>Welcome to the next-gen baby!</t>
+  </si>
+  <si>
+    <t>First 5G phone. Another addition to list of great innovations by Samsung. And yeah, first actual foldable phone too.</t>
+  </si>
+  <si>
+    <t>Droid, 15 hours agoThis will be the phone to beat in 2019._x000D_
+Inanse screen and battery sizeAgreed. I'm excited to see what Huawei brings with the P30.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">big dimensions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not a good size for a phone . It should be little bigger then this because it's a tablet   . Like the size of mi Max 4. </t>
+  </si>
+  <si>
+    <t>This will be the phone to beat in 2019. _x000D_
+Inanse screen and battery size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="3">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,26 +147,42 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -383,18 +470,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -414,17 +495,305 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43517</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C21" r:id="rId20"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes done in view and gsmarena get issue
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Product</t>
   </si>
@@ -27,25 +27,12 @@
   <si>
     <t>comment</t>
   </si>
-  <si>
-    <t>Asus Zenfone Max (M1) ZB556KL</t>
-  </si>
-  <si>
-    <t>02/09/2019</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/asus_zenfone_max_(m1)_zb556kl-reviews-9373.php</t>
-  </si>
-  <si>
-    <t>Kamal, 28 Dec 2018Humen reached at moon but i can not read these asus phones name._x000D_
-Go at shop and ask asus Wj12... moreJust say Zenfone Max (M1)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +47,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,22 +81,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -429,24 +403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Keyward Code and SQLDB code
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>Product</t>
   </si>
@@ -45,57 +45,283 @@
   </si>
   <si>
     <t xml:space="preserve">
-emornet
+azzido
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Veteran</t>
+  </si>
+  <si>
+    <t>Ram,Headphone Jack,Battery,</t>
+  </si>
+  <si>
+    <t>Xperia 1 availability</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Xperia-1-availability/td-p/1365311/page/4</t>
+  </si>
+  <si>
+    <t>2019-04-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@Aderaldo-23 wrote:SONY is taking so long to this sales date that I'm willing to think that its strategy is to release an Xperia 1 "version 2" including much more good surprises. Would be great to have it with 8GB of RAM, more ROM, 4000mAh+ battery and headphone jack! 
+</t>
+  </si>
+  <si>
+    <t>Sensor,Screen,Power button,Power,Battery,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@Andross01 wrote:Maybe the problem is again some exclusive Samsung-Qualcomm deal that also happened with the XZ Premium. The flagship Snapdragon CPU was not available for mass production for other manufacturers other than Samsung back then in March-May 2017. Or Sony takes a little while longer to check what issues people come up with to not buy the Xperia 1 (no wireless charging, finger print sensor and power button separated, not enough battery power, etc.) to make the phone truly perfect.This time snapdragon availability should not be the case since sony participated in developing it with qualcomm! It should be clocked higher and be faster on sony. And there are already other brands than shamesung with devices on snap 855 hence it seems it ia not the case. I hope screen will be brighter than what was shown. Current x1 was less bright than xz3 os shame s9 
+</t>
+  </si>
+  <si>
+    <t>Ram,Battery,</t>
+  </si>
+  <si>
+    <t>Is there an official price yet?</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Is-there-an-official-price-yet/td-p/1367340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It should be less considering the specs, they offer less than other flagships (ram, rom, battery, jack) and asking same price... They offer budget s10e specs in price of s10+ :/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+FakeID
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rookie</t>
+  </si>
+  <si>
+    <t>Screenshot,Lock,</t>
+  </si>
+  <si>
+    <t>2019-04-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@azzido I think the curved building photo it's form wide-angle lens on xperia 1, distortion it's acceptable, also in one  screenshot shows there is a distortion control option(chinese), he turn to "Prioritize distortion correction", probably turn off when he took that photo. can't reply you in original post,it's lock.        
+</t>
+  </si>
+  <si>
+    <t>Touch,Screen,Photos,Performance,Google,Display,Camera,</t>
+  </si>
+  <si>
+    <t>Xperia 1 photo sample and some experience</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Xperia-1-photo-sample-and-some-experience/td-p/1369340</t>
+  </si>
+  <si>
+    <t>2019-04-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Someone post on weibo ，He said some experience as follows （Google Translate）1.game mode prompts a lot of performance and execution efficiency2.screen display is amazing , brightness is not bright than XZ33.improved touch performance4.open camera API, you can bin out the google camera,use opencamera with 4K 60FPS 100mbps5.photo  is obviously improved，photo algorithm more like RX100 II，hdr improved but not stable6.import raw from lightroom belongs to the first class "mobilephone camp" He has deleted the post for some reason， no full size photos sharing。    
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+uliwooly
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Emperor</t>
+  </si>
+  <si>
+    <t>Performance,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@FakeID  @azzido  I'm sure we are eagerly anticipating getting our hands on this device and play with/test it; But, we still a bit more than a month ahead. Perhaps some user got a hold of a Xperia 1; even if someone did, he/she probably got his/her hands on either a prototype Xperia 1 or not the final software, who knows, unless that user has more info/proof, we can only speculate, and that will side track the topic of this post.  Based from what you've posted it seems like an amazing device, can't wait to see the final product and its performance.
+"I'd rather be hated for who I am, than loved for who I am not." Kurt Cobain (1967-1994)
+</t>
+  </si>
+  <si>
+    <t>Screen,Photos,Abnormal,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Indeed brightness of the screen is worse than xz3 or shamesung s9 which is very bad  Look at some photos with buildings!It looks like abnormal distortion issue is back!!!!  !! ! !! !!!!!!!  ! !!!!!!!!!!! ! !! !! 😭 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+bb25
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visitor</t>
+  </si>
+  <si>
+    <t>Headset,Headphone Jack,</t>
+  </si>
+  <si>
+    <t>Headphone jack compatible! Xperia 1</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Headphone-jack-compatible-Xperia-1/td-p/1369443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Look at the compatibility list!Headphone jack compatible!Stereo Headset STH32https://www.sonymobile.com/global-en/products/accessories/#filter=.compatibility-xperia1 
+</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@bb25  Thanks for the heads up, I'll escalate this. 
+"I'd rather be hated for who I am, than loved for who I am not." Kurt Cobain (1967-1994)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Jonas
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sony Xperia Support</t>
+  </si>
+  <si>
+    <t>USB,Touch,Headset,Headphone Jack,Accessory,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hi @bb25,As far as I know, the Xperia 1 box will include the adapter (3.5 mm to USB Type-C) that has been included in the box for all our other devices that does not have a headphone jack, so it's still possible to use the STH32 or any other wired headset with the Xperia 1 (or any other Xperia devices that does not have a headphone jack).The STH32 is listed as an accessory for the Xperia XZ3 as well.https://www.sonymobile.com/global-en/products/phones/xperia-xz3/accessories/Let me know if anything is unclear! 
+Official Sony Xperia Support StaffIf you're new to our forums, make sure that you've read our Discussion guidelines.To get in touch with your local support team, please visit our contact page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+sonyuser8
 </t>
   </si>
   <si>
     <t xml:space="preserve"> One time poster</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Xperia 1 Compact</t>
-  </si>
-  <si>
-    <t>https://talk.sonymobile.com/t5/Xperia-1/Xperia-1-Compact/td-p/1364920/page/2</t>
-  </si>
-  <si>
-    <t>2019-03-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I also had 3 different Xperia compact version. The X compact I'm still using is really perfect in many points... And for the first time since my Ericsson T10s, the lack of Xperia One Compact will force me to leave Sony. The only last plus you had in this tough mobile phone market was the compact top version ... Your choice is hard to understand. I imagine reading all comment, that many People like me can't imagine themseseves using à quasi IPad to Have à Phone call !!
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Sensination
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Commissioner</t>
-  </si>
-  <si>
-    <t>Who is excited for the 1?</t>
-  </si>
-  <si>
-    <t>https://talk.sonymobile.com/t5/Xperia-1/Who-is-excited-for-the-1/td-p/1366018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I am now but I won't be anymor ein June... Also by that time Galaxy S10 will cost 70% of what X1 will cost....
-</t>
-  </si>
-  <si>
-    <t>['App', 'Bluetooth', 'Ram', 'Screen']</t>
-  </si>
-  <si>
-    <t>https://talk.sonymobile.com/t5/Xperia-1/Xperia-1/td-p/1364873/page/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1. No thanks, I prefer to use my €1,000 headphones that use jack rather than buying sub-par bluetooth kids toys. 3. I never used multitasking and I see no reason to have such tall screen on the phone. Of course it's my opinion and I know that some people will ike it some will hate it. 4. I see that you have never seen 4k 60fps vidoe? If you have you'd understand why 24fps or 30fps looks rubbish in comparison to 60fps. My wife has iPhone XS which can record 4k 60 fps and the enjoymrnt from watching the 60fps videos is much much better. 5. No, they are just to cheap to pay for the patent.  10. Have you ever used a phone with 8GB or 10GB RAM? I have and the difference is huge. Xperia has awful RAM management and my XZ3 closes even small apps like crazy. My firiend's Huawei keeps even big games open. If I open maps and one more app when watching Netflix, Xperia kills it? Seriously? You are completely wron 6GB is a bare MINIMUM for mid-range phones these days...
+    <t>Screen,Headphone Jack,Display,Camera,</t>
+  </si>
+  <si>
+    <t>Bring back the headphone jack!!!</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Bring-back-the-headphone-jack/td-p/1369140</t>
+  </si>
+  <si>
+    <t>2019-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hello, I'd like to express my disappointment that Sony has abandoned its typical design (dedicated camera button + 3.5mm headphone jack + bezels) which made it stand out and now follows the trend of pointless changes by dropping the headphone jack in flagships or the camera button in mid-range devices - providing solutions that seek to solve problems which don't even exist! The 21:9 display seems logical idea for multitasking and I support it (although it would be nice to have various display ratio options). In my opinion forcing customers to choose either a dedicated camera button or a 3.5mm headphones jack in the latest smartphones line (Xperia 1, 10, 10 Plus) is the first step of Sony losing its identity and blindly imitating others. I believe there are lots of people, who like me hate notches/punch-holes, rounded display corners (which take away screen area) and bezelless designs (which make holding the phone difficult without covering the display with hands). I hope that other fans will also join and take the time to express their frustration with the latest changes and make Sony design teams listen. Otherwise we'll quietly vote with our wallets. I hope this helps Sony to revise its designs for future models. Thank you.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Oh look at the compatibility list!Headphone jack compatible!Stereo Headset STH32https://www.sonymobile.com/global-en/products/accessories/#filter=.compatibility-xperia1 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@bb25  That's a mistake @bb25  @sonyuser8 only the Xperia 10 and 10 Plus are 3.5mm compatible. I already escalated that. 
+"I'd rather be hated for who I am, than loved for who I am not." Kurt Cobain (1967-1994)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Zackbuks
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Regular</t>
+  </si>
+  <si>
+    <t>Vibration,Google Play,Google,Feature,</t>
+  </si>
+  <si>
+    <t>Can you guys put the Xperia Actions back?</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Can-you-guys-put-the-Xperia-Actions-back/td-p/1369420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I've used the Xperia Actions from Xperia XZ Premium and its Focus/Sleep Mode is very useful to daily life. I know the Android has disturb mode but it can't switch the phone to Vibration. And the Xperia Actions is the only unique feature of Xperia to myself.Since Sony dropped it on the Xperia XZ3 I felt lots of inconvenience but somehow there is a pure version so I can install it on XZ3/10 Plus and works well.But I still hope the Sony Mobile can put it back or just make a public version on Google Play to make this feature popular.I want to buy the Xperia  1 with/without feature, but I truly want this feature back through.#Xperia1 
+</t>
+  </si>
+  <si>
+    <t>Touch,</t>
+  </si>
+  <si>
+    <t>XPERIA phone update</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/XPERIA-phone-update/td-p/1367170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@AndyCalling, haha, yeah, it's very confusing and I'm not really sure how everyone will be impacted by this or if it is the standard panic and in the end, it's barely a difference if you are in or out of the EU. I should probably read up on it, just need to find some good source. I can also promise you that I'm not David Cameron! Have a great Monday!
+Official Sony Xperia Support StaffIf you're new to our forums, make sure that you've read our Discussion guidelines.To get in touch with your local support team, please visit our contact page.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Strampke
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pioneer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Not that it has anything to do with the subject but GB nowadays has a great resemblance with the latest work of art of Banksey.Your all moving in the same direction more or less and on your way you're spliting up, resulting in the destruction of this work of art.Which in itself can be a new work of art depending how one appreciates the outcome. Grumph, strange guys those Britts, strange guys, grumph
+who knows knowswho doesn't doesn't 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Janine39
+</t>
+  </si>
+  <si>
+    <t>Help please trash Bin?where  can i find it</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Help-please-trash-Bin-where-can-i-find-it/td-p/1369150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+When you deleted files is it totaly disappeared? Or  the deleted files goes to any trash bin? Does  SonyXperia  phone has a trash bin?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+skycamefalling
+</t>
+  </si>
+  <si>
+    <t>System,Gallery,Functionality,Feature,App,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+There is no general system-wide trashbin.Usually when you delete a file it's gone.However, it depends on the app you are using to delete something. There are several file managers in the store that have a trashbin function (I'm using File Commander, for example). There are also photo gallery apps with such a feature. So a trashbin-functionality is possible but is has to be implemented in the app you are using to delete a specific file.
+</t>
+  </si>
+  <si>
+    <t>Touch,Album,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hi @Janine39, welcome to our forum!@skycamefalling pretty much covered it all! As per standard there is no trash bin/recycle bin in Android devices, but some applications may have one available.As far as I know, you need to delete the file using this application to be able to recover it, so for example, if you delete a photo in the Album application, it will not show up in the trash bin in for example, File Commander. @skycamefalling can probably confirm or deny this though! Have a nice day!
+Official Sony Xperia Support StaffIf you're new to our forums, make sure that you've read our Discussion guidelines.To get in touch with your local support team, please visit our contact page.
 </t>
   </si>
 </sst>
@@ -445,7 +671,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,25 +736,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -536,25 +762,467 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
       <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Dashboard with Prod Selection Button
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Product</t>
   </si>
@@ -32,66 +32,41 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Samsung Galaxy S10 5G</t>
-  </si>
-  <si>
-    <t>04/09/2019</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/samsung_galaxy_s10_5g-reviews-9588p1.php</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>No doubt this is the best choice</t>
-  </si>
-  <si>
-    <t>Akuma, 08 Apr 20195G has rolled out in Korea already.Yes. Very fast.</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S10+</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/samsung_galaxy_s10+-reviews-9535p1.php</t>
-  </si>
-  <si>
-    <t>Power,Photos,Media,Battery,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Android Boy, 09 Apr 2019Hi.
-I'm thinking of buying this phone or the Huawei P30 pro. I'm a bit concerned with the bat... morehmm...  from my experience.  been a samsung fan since... well basically forever. lol. one thing i always complain is battery tbh. im on their Note and casually tries their S, what i observe, i dunno for others all right, dont take this as absolute truth buddy. what i observed is that well after several months i keep i having battery drain issues. every purchase, thats my only complain everytime. i am not the one who tinkers on my phone. last year, my note 8 disappointed me big time, when i needed it the most in the office it just shut down because of low power, its not even that low batt and i have to charge it to be able to switch it on.  thats the reason i skipped last years note, i was just basically full of it. tried an apple xs last year as an alternative bwehh.. after less than a month i sold to my office mate. i cant handle ios tbh. then i heard this poco frenzy going on, tried it. after few days i sold, look cheap for my liking tbh. then after a "decade" lol, of finding the one that best suit my battery needs, i settled with mate 20 pro, its quite excellent with battery life tbh. its one of the reason i skipped s10, its battery really is good. the other reason being the note 10. i hope it doesnt disappoint. i will be switching to note 10 this year or if mate 30 have something good to offer, ill bite since that brand already got my trust anyways.
-not a heavy user too. im jusing my phone majority for work, photos/videos and social media. no games, not a gamer. </t>
-  </si>
-  <si>
-    <t>Battery,</t>
-  </si>
-  <si>
-    <t>Hi. 
-I'm thinking of buying this phone or the Huawei P30 pro. I'm a bit concerned with the battery. Those who have the Exynos model, can say if is true about the battery drain, or the battery is good? I'm not a heavy user. I only use the phone to check email, Facebook, some web pages and that is all. Thanks</t>
-  </si>
-  <si>
-    <t>realitychecker, 07 Apr 2019kind of whats happening here in our office. used to have many samsung users, now not even one ... moreMe too.</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S10</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/samsung_galaxy_s10-reviews-9536p1.php</t>
-  </si>
-  <si>
-    <t>Mohamed imran, 09 Apr 2019Hi,
-Pls let me know about battery.
-While charged 100% battery it reduced to 98% with in 10 t... moreIts happening on my S10+ too that I bought 5 days ago.</t>
-  </si>
-  <si>
-    <t>Screen,Battery,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi, 
-Pls let me know about battery. 
-While charged 100% battery it reduced to 98% with in 10 to 15 mins without any usage.  (Not even screen wake up) 
-It's nornal for S10 or battery issue?
+    <t>Samsung Galaxy M30</t>
+  </si>
+  <si>
+    <t>04/11/2019</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/samsung_galaxy_m30-reviews-9505p1.php</t>
+  </si>
+  <si>
+    <t>NFC,Fm Radio,</t>
+  </si>
+  <si>
+    <t>M30 does not have gorilla glass, FM radio and NFC. A useless, worthless model.
+Samsung A9 2018 is far more better than M30 and A50
+A50 has gorilla glass 3 but does not have NFC and FM radio.
+Samsung is digging its own grave. Even Samsung A9 pro 2016 and other models have gorilla glass, FM radio and NFC</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M20</t>
+  </si>
+  <si>
+    <t>https://www.gsmarena.com/samsung_galaxy_m20-reviews-9506p1.php</t>
+  </si>
+  <si>
+    <t>Video,Update,</t>
+  </si>
+  <si>
+    <t>Anonymous, 9 hours agoHello im having  heating issu after the latest update and i chat with samsung support and they... moreWhy bro , they can't help? definitely they should help if your mobile phone doesn't have any physical damage. 
+Try for second time (that time take a note about about the staff what they saying better you record a video and send email with the video to Samsung main head office - Korea regarding about the issue) they definitely help you, don't worry.</t>
+  </si>
+  <si>
+    <t>Update,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello im having  heating issu after the latest update and i chat with samsung support and they tell me go to the service center and the service center cant help me what can i do .
 </t>
   </si>
 </sst>
@@ -441,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,104 +460,36 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Google Charts Dashboard for Sony Forum
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -20,53 +20,53 @@
     <t>Product</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Thread</t>
+    <t>First User Name</t>
+  </si>
+  <si>
+    <t>Second User Name</t>
   </si>
   <si>
     <t>Category</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy M30</t>
-  </si>
-  <si>
-    <t>04/11/2019</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/samsung_galaxy_m30-reviews-9505p1.php</t>
-  </si>
-  <si>
-    <t>NFC,Fm Radio,</t>
-  </si>
-  <si>
-    <t>M30 does not have gorilla glass, FM radio and NFC. A useless, worthless model.
-Samsung A9 2018 is far more better than M30 and A50
-A50 has gorilla glass 3 but does not have NFC and FM radio.
-Samsung is digging its own grave. Even Samsung A9 pro 2016 and other models have gorilla glass, FM radio and NFC</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy M20</t>
-  </si>
-  <si>
-    <t>https://www.gsmarena.com/samsung_galaxy_m20-reviews-9506p1.php</t>
-  </si>
-  <si>
-    <t>Video,Update,</t>
-  </si>
-  <si>
-    <t>Anonymous, 9 hours agoHello im having  heating issu after the latest update and i chat with samsung support and they... moreWhy bro , they can't help? definitely they should help if your mobile phone doesn't have any physical damage. 
-Try for second time (that time take a note about about the staff what they saying better you record a video and send email with the video to Samsung main head office - Korea regarding about the issue) they definitely help you, don't worry.</t>
-  </si>
-  <si>
-    <t>Update,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello im having  heating issu after the latest update and i chat with samsung support and they tell me go to the service center and the service center cant help me what can i do .
+    <t>Thread Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Links </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Issue Detail</t>
+  </si>
+  <si>
+    <t>Xperia 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Jonas
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sony Xperia Support</t>
+  </si>
+  <si>
+    <t>Touch,</t>
+  </si>
+  <si>
+    <t>Fast Charger UCH32C</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/Fast-Charger-UCH32C/td-p/1370427</t>
+  </si>
+  <si>
+    <t>2019-04-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hi @pressefr!Do I understand correctly if you want to know if this charger will be included in box content for the Xperia 1 in the US? If that is correct, this is very tricky for me to answer here at our Global user based forum as the box content is different, not only between markets, but can also be different depending on the retailer from where the device is bought.The UCH32C charger is not listed on the Sony Mobile website for the US, but you may want to get in touch with the Local support team there and see if they have any additional information, not only regarding the availability, but also the box content for the Xperia 1, in their market.Feel free to let me know if you are able to get some information about this from them, as I'm sure there are other users from the US that are also interested in knowing this! 
+Official Sony Xperia Support StaffIf you're new to our forums, make sure that you've read our Discussion guidelines.To get in touch with your local support team, please visit our contact page.
 </t>
   </si>
 </sst>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,55 +440,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Google Chart Code Changed to Apply Date Sort Order
</commit_message>
<xml_diff>
--- a/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
+++ b/SocialMediaIssueTrackingTool/ScrapingTool/files/FinalData.xlsx
@@ -837,8 +837,145 @@
 </t>
   </si>
   <si>
+    <t>Recording,</t>
+  </si>
+  <si>
+    <t>That camera though 😍😍😍</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/That-camera-though/td-p/1364869/page/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Can't wait to play with that CineAlta recording.21:9 OIS 4k HDR using LOOK and tuned by cine alta...Drooling I tell you, drooling!
+Moderators are not affiliated with, or work for Sony Mobile, and their posts represent their own opinions and views.Click here to find out more about the different roles on the community.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+diogosimoes4321
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@viridis i can also wait to see the new BionzX for mobile to see how improves compared to the old version! It was about time! 
+	_______________Diogo SimõesThis is a user-based global forum. So please, write in english! By doing so, it can be well received and monitored.If the problem is solved, mark it as a solution so others can know 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+This is the spec equivalent....That is off the charts nice.Anything near this will be absolute lush https://youtu.be/_2SycQCIPt0
+Moderators are not affiliated with, or work for Sony Mobile, and their posts represent their own opinions and views.Click here to find out more about the different roles on the community.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I'm a cinematographer using the A7SII and FS5 at the moment and I would love to make a short film using this as proof of concept  Please can I have a pre-release model to do that? 
+</t>
+  </si>
+  <si>
+    <t>Sensor,Camera,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Camera set up looks really good but I was hoping that there would be an ultra wide and that the 50 mp sensor rumors were true.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Ted05
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inhabitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Thanks for posting the Xperia 1 camera specs - it looks brilliant!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brian_gjx
+</t>
+  </si>
+  <si>
+    <t>Photos,Camera,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I'm excited about the camera too! Especially alpha team is involved this time. Btw, someone on other thread asking it seems 3 out of 4 camera sensors on this device are non-Sony made.Even if it's true, Im fine as long as it can take good photos, but I just want to know. Anyone has answer to this question?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Posie19
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Xperia 1 camera has: triple lens12-megapixel sensorswide lens with optical image stabilisation, telephoto lens and super wide lensAlpha certificationeye tracking autofocus videoability to film in 24fps at 21:9  What's not to love?!
+</t>
+  </si>
+  <si>
+    <t>Video,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Without 4k 60FPS option it's a complete joke! What's the point of releasing a phone directed at video making enthusiasts without it? Snapdragon 845 can already handle it so why can't we have it in a phone with Snapdragon 855?? Another half baked phone from Sony. Two steps forward, three steps backward as usual...
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 ds2mph
+</t>
+  </si>
+  <si>
+    <t>2019-04-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Most people will use more 4K@60fps SDR recording than 4K@24fps 21:9 HDR recording, Sony!!! Why does Sony not  provide 4K@60fps recording???? Again, disappointment... Maybe Sony Camcorder team do not want to give a help to Xperia
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Stalker777
+</t>
+  </si>
+  <si>
+    <t>Youtube,Picture,Camera,</t>
+  </si>
+  <si>
+    <t>https://talk.sonymobile.com/t5/Xperia-1/That-camera-though/td-p/1364869/page/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+It seems that even God himself, will not be able to teach the XPERIA camera to shoot so that both the foreground and the background are in harmony with each other.As we can see here, the background in the picture is overexposed!. Sony does not know how to make a camera, as competitors successfully do.https://ibb.co/6HMGD2y, the same  https://ibb.co/Qk0dn08Why users must selling XZ2 and buying this one? Only for 2x zoom?  https://www.youtube.com/watch?v=2LKwOOEGtrgThis is old story. Xperia can show ballance, even in manualhttps://youtu.be/8yovUwlz_VA?t=120DXO test XZ3 https://cdn.dxomark.com/wp-content/uploads/medias/post-27511/BridgeHDR_SonyXperiaXZ3_DxOMark_05-00.j...   The same (( Sony smartphone cameras always was weack in high-contrast scenes  https://ibb.co/F8Q5nVghttps://ibb.co/TmWVF6XThe camera shoots the same, with the same of overexpose background and pale color Thermometer_Face:
+</t>
+  </si>
+  <si>
+    <t>Recording,Performance,Hardware,Camera,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@Posie19 wrote:Xperia 1 camera has: triple lens12-megapixel sensorswide lens with optical image stabilisation, telephoto lens and super wide lensAlpha certificationeye tracking autofocus videoability to film in 24fps at 21:9  What's not to love?!Probably I will not love the night performance will be worse than p30 pro, since x1 is using shamesung's LAST YEAR, hence s9 camera modules and even s10 is much worse at night than p30 pro. I will not like lack of 4k 60fps either... Instead we will have a regres like recording in... 24fps...so we will have a slideshow. So called cinematic experience from the consoles (lack of 60fps due to crappy hardware) in Xperias. But snap 855 is capable of 4k 60fps recording, it's sony that doesn't want to give it to us (as usually). Can't wait for cine alta slideshows! 
+</t>
+  </si>
+  <si>
+    <t>Sensor,Ram,Camera,Battery,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+I also do not understand why x1 is coming with inferior technology of only 2x optical zoom while p30 pro already has 5x optical zoom, 10x hybrid and 50x digital... And is already on the market.And this telephoto sensor has more megapixels and better aperture.  Even front camera of x1 looks like a regres, my old xz premium has 13mpx front camera and x1 is coming with 8mpx  f2.0 sensor. I will likely buy x1 to support sony but this time I am not so sure of it. They are coming with outdated specs 6GB of RAM vs 8 at competition, worse camera, much smaller battery, also li ion vs li polymer, li-ion used by sony is cheaper). And it is coming so late to the party, where true release date is still unknown and we have May!  So I am not that sure why sony wants me to charge 1k $ for X1. Looking at competition and what it offers at this price I am really wondering. 
+</t>
+  </si>
+  <si>
+    <t>2019-05-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Xperia 1 seems to use Carl Zeiss milvus  lenses 
 </t>
   </si>
   <si>
@@ -916,11 +1053,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-diogosimoes4321
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 It´s probably algorithms, just lie Bravia Engine was! 
 	_______________Diogo SimõesThis is a user-based global forum. So please, write in english! By doing so, it can be well received and monitored.If the problem is solved, mark it as a solution so others can know 
 </t>
@@ -931,9 +1063,6 @@
 </t>
   </si>
   <si>
-    <t>Sensor,Camera,</t>
-  </si>
-  <si>
     <t>Does Xperia 1 use Samsung's camera sensor?</t>
   </si>
   <si>
@@ -1028,11 +1157,6 @@
   </si>
   <si>
     <t xml:space="preserve">
-Brian_gjx
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 Jonny got the point. I'm interested too.EUPHORIC, you have not answered his question at all, and it's totally fine.But you should not bend the intention of his question. 
 </t>
   </si>
@@ -1235,9 +1359,6 @@
 </t>
   </si>
   <si>
-    <t>Video,</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Well, I will really make an extensive and beautiful video, hope it gets traction... I wouldn't expect Sony to outsell Samsung, I am aware of the market situation, but couldn't Sony learn from it and do something about it? I also know their semiconductor business is way more important to them, but some steps would be so easy...- A more relatable and exciting product unveiling with immediate availability- Tighter integration with successful products from the company (PS, cameras, headphones. .) including bundles...- Product placement with so many Sony film and music releases. I know some things are out of control, but marketing and releasing a phone with huge bezels in a bezelless world are just wrong steps. 
 </t>
@@ -1306,127 +1427,6 @@
   <si>
     <t xml:space="preserve">
 @Diamanj wrote:Very disappointed in this release. I was hoping to replace my P20 Pro. I had read early reports about 52MP and 4000 battery, I was in. Now with 12MP and 3333 Battery I'm out.Yeah, I was hyped for this 52MPx main camera and 4000mAh+ battery too. The only confirmed from the early reports is price while the others... 
-</t>
-  </si>
-  <si>
-    <t>Recording,</t>
-  </si>
-  <si>
-    <t>That camera though 😍😍😍</t>
-  </si>
-  <si>
-    <t>https://talk.sonymobile.com/t5/Xperia-1/That-camera-though/td-p/1364869/page/1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Can't wait to play with that CineAlta recording.21:9 OIS 4k HDR using LOOK and tuned by cine alta...Drooling I tell you, drooling!
-Moderators are not affiliated with, or work for Sony Mobile, and their posts represent their own opinions and views.Click here to find out more about the different roles on the community.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-@viridis i can also wait to see the new BionzX for mobile to see how improves compared to the old version! It was about time! 
-	_______________Diogo SimõesThis is a user-based global forum. So please, write in english! By doing so, it can be well received and monitored.If the problem is solved, mark it as a solution so others can know 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-This is the spec equivalent....That is off the charts nice.Anything near this will be absolute lush https://youtu.be/_2SycQCIPt0
-Moderators are not affiliated with, or work for Sony Mobile, and their posts represent their own opinions and views.Click here to find out more about the different roles on the community.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I'm a cinematographer using the A7SII and FS5 at the moment and I would love to make a short film using this as proof of concept  Please can I have a pre-release model to do that? 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Camera set up looks really good but I was hoping that there would be an ultra wide and that the 50 mp sensor rumors were true.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Ted05
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Inhabitant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Thanks for posting the Xperia 1 camera specs - it looks brilliant!
-</t>
-  </si>
-  <si>
-    <t>Photos,Camera,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I'm excited about the camera too! Especially alpha team is involved this time. Btw, someone on other thread asking it seems 3 out of 4 camera sensors on this device are non-Sony made.Even if it's true, Im fine as long as it can take good photos, but I just want to know. Anyone has answer to this question?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Posie19
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Xperia 1 camera has: triple lens12-megapixel sensorswide lens with optical image stabilisation, telephoto lens and super wide lensAlpha certificationeye tracking autofocus videoability to film in 24fps at 21:9  What's not to love?!
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Without 4k 60FPS option it's a complete joke! What's the point of releasing a phone directed at video making enthusiasts without it? Snapdragon 845 can already handle it so why can't we have it in a phone with Snapdragon 855?? Another half baked phone from Sony. Two steps forward, three steps backward as usual...
-</t>
-  </si>
-  <si>
-    <t>2019-04-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Most people will use more 4K@60fps SDR recording than 4K@24fps 21:9 HDR recording, Sony!!! Why does Sony not  provide 4K@60fps recording???? Again, disappointment... Maybe Sony Camcorder team do not want to give a help to Xperia
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Stalker777
-</t>
-  </si>
-  <si>
-    <t>Youtube,Picture,Camera,</t>
-  </si>
-  <si>
-    <t>https://talk.sonymobile.com/t5/Xperia-1/That-camera-though/td-p/1364869/page/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-It seems that even God himself, will not be able to teach the XPERIA camera to shoot so that both the foreground and the background are in harmony with each other.As we can see here, the background in the picture is overexposed!. Sony does not know how to make a camera, as competitors successfully do.https://ibb.co/6HMGD2y, the same  https://ibb.co/Qk0dn08Why users must selling XZ2 and buying this one? Only for 2x zoom?  https://www.youtube.com/watch?v=2LKwOOEGtrgThis is old story. Xperia can show ballance, even in manualhttps://youtu.be/8yovUwlz_VA?t=120DXO test XZ3 https://cdn.dxomark.com/wp-content/uploads/medias/post-27511/BridgeHDR_SonyXperiaXZ3_DxOMark_05-00.j...   The same (( Sony smartphone cameras always was weack in high-contrast scenes  https://ibb.co/F8Q5nVghttps://ibb.co/TmWVF6XThe camera shoots the same, with the same of overexpose background and pale color Thermometer_Face:
-</t>
-  </si>
-  <si>
-    <t>Recording,Performance,Hardware,Camera,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-@Posie19 wrote:Xperia 1 camera has: triple lens12-megapixel sensorswide lens with optical image stabilisation, telephoto lens and super wide lensAlpha certificationeye tracking autofocus videoability to film in 24fps at 21:9  What's not to love?!Probably I will not love the night performance will be worse than p30 pro, since x1 is using shamesung's LAST YEAR, hence s9 camera modules and even s10 is much worse at night than p30 pro. I will not like lack of 4k 60fps either... Instead we will have a regres like recording in... 24fps...so we will have a slideshow. So called cinematic experience from the consoles (lack of 60fps due to crappy hardware) in Xperias. But snap 855 is capable of 4k 60fps recording, it's sony that doesn't want to give it to us (as usually). Can't wait for cine alta slideshows! 
-</t>
-  </si>
-  <si>
-    <t>Sensor,Ram,Camera,Battery,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-I also do not understand why x1 is coming with inferior technology of only 2x optical zoom while p30 pro already has 5x optical zoom, 10x hybrid and 50x digital... And is already on the market.And this telephoto sensor has more megapixels and better aperture.  Even front camera of x1 looks like a regres, my old xz premium has 13mpx front camera and x1 is coming with 8mpx  f2.0 sensor. I will likely buy x1 to support sony but this time I am not so sure of it. They are coming with outdated specs 6GB of RAM vs 8 at competition, worse camera, much smaller battery, also li ion vs li polymer, li-ion used by sony is cheaper). And it is coming so late to the party, where true release date is still unknown and we have May!  So I am not that sure why sony wants me to charge 1k $ for X1. Looking at competition and what it offers at this price I am really wondering. 
-</t>
-  </si>
-  <si>
-    <t>2019-05-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Xperia 1 seems to use Carl Zeiss  lenses 
 </t>
   </si>
   <si>
@@ -6020,13 +6020,13 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" t="s">
+        <v>174</v>
+      </c>
+      <c r="D75" t="s">
         <v>199</v>
-      </c>
-      <c r="C75" t="s">
-        <v>35</v>
-      </c>
-      <c r="D75" t="s">
-        <v>18</v>
       </c>
       <c r="E75" t="s">
         <v>200</v>
@@ -6035,7 +6035,7 @@
         <v>201</v>
       </c>
       <c r="G75" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H75" t="s">
         <v>202</v>
@@ -6049,7 +6049,7 @@
         <v>203</v>
       </c>
       <c r="C76" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="D76" t="s">
         <v>18</v>
@@ -6061,7 +6061,7 @@
         <v>201</v>
       </c>
       <c r="G76" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H76" t="s">
         <v>204</v>
@@ -6072,25 +6072,25 @@
         <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="C77" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="E77" t="s">
+        <v>200</v>
+      </c>
+      <c r="F77" t="s">
+        <v>201</v>
+      </c>
+      <c r="G77" t="s">
+        <v>197</v>
+      </c>
+      <c r="H77" t="s">
         <v>205</v>
-      </c>
-      <c r="F77" t="s">
-        <v>206</v>
-      </c>
-      <c r="G77" t="s">
-        <v>207</v>
-      </c>
-      <c r="H77" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -6098,25 +6098,25 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>209</v>
+        <v>16</v>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="D78" t="s">
         <v>18</v>
       </c>
       <c r="E78" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F78" t="s">
+        <v>201</v>
+      </c>
+      <c r="G78" t="s">
+        <v>197</v>
+      </c>
+      <c r="H78" t="s">
         <v>206</v>
-      </c>
-      <c r="G78" t="s">
-        <v>127</v>
-      </c>
-      <c r="H78" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -6124,25 +6124,25 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="C79" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D79" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E79" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F79" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G79" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="H79" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -6150,25 +6150,25 @@
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
-        <v>213</v>
+        <v>116</v>
       </c>
       <c r="E80" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F80" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G80" t="s">
-        <v>181</v>
+        <v>61</v>
       </c>
       <c r="H80" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -6176,25 +6176,25 @@
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>82</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="D81" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E81" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F81" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G81" t="s">
-        <v>216</v>
+        <v>61</v>
       </c>
       <c r="H81" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -6202,25 +6202,25 @@
         <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C82" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D82" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="E82" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F82" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G82" t="s">
+        <v>84</v>
+      </c>
+      <c r="H82" t="s">
         <v>216</v>
-      </c>
-      <c r="H82" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -6228,25 +6228,25 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>220</v>
+        <v>29</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D83" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E83" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F83" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="G83" t="s">
-        <v>224</v>
+        <v>134</v>
       </c>
       <c r="H83" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -6254,25 +6254,25 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="C84" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>199</v>
       </c>
       <c r="E84" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F84" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="G84" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H84" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -6280,25 +6280,25 @@
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>56</v>
+        <v>222</v>
       </c>
       <c r="C85" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="D85" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E85" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F85" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G85" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="H85" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -6306,25 +6306,25 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D86" t="s">
-        <v>18</v>
+        <v>226</v>
       </c>
       <c r="E86" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F86" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G86" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="H86" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -6332,25 +6332,25 @@
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D87" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E87" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F87" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G87" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="H87" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -6358,25 +6358,25 @@
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
       </c>
       <c r="D88" t="s">
-        <v>232</v>
+        <v>18</v>
       </c>
       <c r="E88" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="F88" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G88" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="H88" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -6384,22 +6384,22 @@
         <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>56</v>
+        <v>219</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D89" t="s">
+        <v>18</v>
+      </c>
+      <c r="E89" t="s">
         <v>232</v>
       </c>
-      <c r="E89" t="s">
-        <v>222</v>
-      </c>
       <c r="F89" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G89" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="H89" t="s">
         <v>234</v>
@@ -6410,25 +6410,25 @@
         <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="C90" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="D90" t="s">
-        <v>221</v>
+        <v>18</v>
       </c>
       <c r="E90" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F90" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G90" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="H90" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -6436,25 +6436,25 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>56</v>
+        <v>219</v>
       </c>
       <c r="C91" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D91" t="s">
-        <v>221</v>
+        <v>156</v>
       </c>
       <c r="E91" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F91" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G91" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="H91" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -6462,25 +6462,25 @@
         <v>8</v>
       </c>
       <c r="B92" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="C92" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="D92" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" t="s">
         <v>237</v>
       </c>
-      <c r="E92" t="s">
-        <v>222</v>
-      </c>
       <c r="F92" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G92" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="H92" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -6488,25 +6488,25 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C93" t="s">
         <v>30</v>
       </c>
       <c r="D93" t="s">
+        <v>243</v>
+      </c>
+      <c r="E93" t="s">
         <v>237</v>
       </c>
-      <c r="E93" t="s">
-        <v>222</v>
-      </c>
       <c r="F93" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="G93" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="H93" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -6514,25 +6514,25 @@
         <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="C94" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D94" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E94" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F94" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G94" t="s">
-        <v>61</v>
+        <v>181</v>
       </c>
       <c r="H94" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -6540,25 +6540,25 @@
         <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>243</v>
+        <v>82</v>
       </c>
       <c r="C95" t="s">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="D95" t="s">
-        <v>18</v>
+        <v>247</v>
       </c>
       <c r="E95" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F95" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G95" t="s">
-        <v>61</v>
+        <v>248</v>
       </c>
       <c r="H95" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -6566,25 +6566,25 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>56</v>
+        <v>203</v>
       </c>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D96" t="s">
-        <v>221</v>
+        <v>18</v>
       </c>
       <c r="E96" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="F96" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G96" t="s">
-        <v>61</v>
+        <v>248</v>
       </c>
       <c r="H96" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -6592,25 +6592,25 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C97" t="s">
-        <v>152</v>
+        <v>35</v>
       </c>
       <c r="D97" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E97" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F97" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G97" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H97" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -6618,25 +6618,25 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>232</v>
+        <v>11</v>
       </c>
       <c r="E98" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F98" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G98" t="s">
-        <v>61</v>
+        <v>256</v>
       </c>
       <c r="H98" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -6644,25 +6644,25 @@
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>243</v>
+        <v>56</v>
       </c>
       <c r="C99" t="s">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="E99" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F99" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G99" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H99" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -6670,25 +6670,25 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="C100" t="s">
         <v>35</v>
       </c>
       <c r="D100" t="s">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="E100" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F100" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G100" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H100" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -6702,19 +6702,19 @@
         <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="E101" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F101" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G101" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H101" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -6722,25 +6722,25 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="C102" t="s">
         <v>35</v>
       </c>
       <c r="D102" t="s">
-        <v>116</v>
+        <v>262</v>
       </c>
       <c r="E102" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F102" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G102" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H102" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -6754,19 +6754,19 @@
         <v>30</v>
       </c>
       <c r="D103" t="s">
-        <v>116</v>
+        <v>262</v>
       </c>
       <c r="E103" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F103" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="G103" t="s">
-        <v>61</v>
+        <v>254</v>
       </c>
       <c r="H103" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -6774,25 +6774,25 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
       <c r="C104" t="s">
         <v>35</v>
       </c>
       <c r="D104" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="E104" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F104" t="s">
+        <v>253</v>
+      </c>
+      <c r="G104" t="s">
         <v>254</v>
       </c>
-      <c r="G104" t="s">
-        <v>61</v>
-      </c>
       <c r="H104" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -6806,19 +6806,19 @@
         <v>30</v>
       </c>
       <c r="D105" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="E105" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F105" t="s">
+        <v>253</v>
+      </c>
+      <c r="G105" t="s">
         <v>254</v>
       </c>
-      <c r="G105" t="s">
-        <v>61</v>
-      </c>
       <c r="H105" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -6826,25 +6826,25 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>9</v>
+        <v>251</v>
       </c>
       <c r="C106" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D106" t="s">
-        <v>11</v>
+        <v>267</v>
       </c>
       <c r="E106" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F106" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G106" t="s">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="H106" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -6858,19 +6858,19 @@
         <v>30</v>
       </c>
       <c r="D107" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="E107" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G107" t="s">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="H107" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -6878,25 +6878,25 @@
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D108" t="s">
-        <v>221</v>
+        <v>270</v>
       </c>
       <c r="E108" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F108" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G108" t="s">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="H108" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -6904,25 +6904,25 @@
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>56</v>
+        <v>212</v>
       </c>
       <c r="C109" t="s">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="D109" t="s">
-        <v>262</v>
+        <v>18</v>
       </c>
       <c r="E109" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F109" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G109" t="s">
-        <v>226</v>
+        <v>61</v>
       </c>
       <c r="H109" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -6930,25 +6930,25 @@
         <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D110" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="E110" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F110" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G110" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H110" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -6956,25 +6956,25 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
-        <v>72</v>
+        <v>212</v>
       </c>
       <c r="C111" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="D111" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="E111" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F111" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G111" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H111" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -6988,19 +6988,19 @@
         <v>30</v>
       </c>
       <c r="D112" t="s">
-        <v>176</v>
+        <v>262</v>
       </c>
       <c r="E112" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F112" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G112" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="H112" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -7008,25 +7008,25 @@
         <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C113" t="s">
-        <v>35</v>
+        <v>152</v>
       </c>
       <c r="D113" t="s">
-        <v>267</v>
+        <v>18</v>
       </c>
       <c r="E113" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F113" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="G113" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="H113" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -7034,25 +7034,25 @@
         <v>8</v>
       </c>
       <c r="B114" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
       <c r="C114" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D114" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="E114" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F114" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G114" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H114" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -7060,25 +7060,25 @@
         <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="C115" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="D115" t="s">
-        <v>18</v>
+        <v>279</v>
       </c>
       <c r="E115" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F115" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G115" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H115" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -7086,25 +7086,25 @@
         <v>8</v>
       </c>
       <c r="B116" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C116" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="D116" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="E116" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F116" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G116" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H116" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -7112,25 +7112,25 @@
         <v>8</v>
       </c>
       <c r="B117" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="C117" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="D117" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="E117" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F117" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G117" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H117" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -7138,25 +7138,25 @@
         <v>8</v>
       </c>
       <c r="B118" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="C118" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D118" t="s">
         <v>18</v>
       </c>
       <c r="E118" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F118" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G118" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H118" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -7164,25 +7164,25 @@
         <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>218</v>
+        <v>56</v>
       </c>
       <c r="C119" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="D119" t="s">
-        <v>18</v>
+        <v>285</v>
       </c>
       <c r="E119" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F119" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G119" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="H119" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -7190,25 +7190,25 @@
         <v>8</v>
       </c>
       <c r="B120" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D120" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="E120" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F120" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G120" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="H120" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -7216,25 +7216,25 @@
         <v>8</v>
       </c>
       <c r="B121" t="s">
-        <v>277</v>
+        <v>56</v>
       </c>
       <c r="C121" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D121" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="E121" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F121" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G121" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="H121" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -7242,25 +7242,25 @@
         <v>8</v>
       </c>
       <c r="B122" t="s">
-        <v>173</v>
+        <v>289</v>
       </c>
       <c r="C122" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="D122" t="s">
-        <v>18</v>
+        <v>207</v>
       </c>
       <c r="E122" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F122" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G122" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="H122" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -7268,25 +7268,25 @@
         <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="C123" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="D123" t="s">
-        <v>83</v>
+        <v>291</v>
       </c>
       <c r="E123" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F123" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="G123" t="s">
-        <v>197</v>
+        <v>256</v>
       </c>
       <c r="H123" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -7294,25 +7294,25 @@
         <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>282</v>
+        <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D124" t="s">
+        <v>18</v>
+      </c>
+      <c r="E124" t="s">
+        <v>252</v>
+      </c>
+      <c r="F124" t="s">
         <v>283</v>
       </c>
-      <c r="E124" t="s">
-        <v>8</v>
-      </c>
-      <c r="F124" t="s">
-        <v>284</v>
-      </c>
       <c r="G124" t="s">
-        <v>197</v>
+        <v>63</v>
       </c>
       <c r="H124" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -7320,25 +7320,25 @@
         <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C125" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D125" t="s">
-        <v>286</v>
+        <v>18</v>
       </c>
       <c r="E125" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F125" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G125" t="s">
-        <v>197</v>
+        <v>70</v>
       </c>
       <c r="H125" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -7346,25 +7346,25 @@
         <v>8</v>
       </c>
       <c r="B126" t="s">
-        <v>173</v>
+        <v>56</v>
       </c>
       <c r="C126" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
       <c r="D126" t="s">
-        <v>18</v>
+        <v>176</v>
       </c>
       <c r="E126" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F126" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G126" t="s">
-        <v>288</v>
+        <v>70</v>
       </c>
       <c r="H126" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -7372,25 +7372,25 @@
         <v>8</v>
       </c>
       <c r="B127" t="s">
-        <v>16</v>
+        <v>219</v>
       </c>
       <c r="C127" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D127" t="s">
-        <v>112</v>
+        <v>296</v>
       </c>
       <c r="E127" t="s">
-        <v>8</v>
+        <v>252</v>
       </c>
       <c r="F127" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G127" t="s">
-        <v>288</v>
+        <v>183</v>
       </c>
       <c r="H127" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -7398,25 +7398,25 @@
         <v>8</v>
       </c>
       <c r="B128" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="C128" t="s">
-        <v>174</v>
+        <v>17</v>
       </c>
       <c r="D128" t="s">
-        <v>291</v>
+        <v>18</v>
       </c>
       <c r="E128" t="s">
         <v>8</v>
       </c>
       <c r="F128" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G128" t="s">
-        <v>288</v>
+        <v>197</v>
       </c>
       <c r="H128" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -7424,25 +7424,25 @@
         <v>8</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>92</v>
       </c>
       <c r="C129" t="s">
-        <v>17</v>
+        <v>93</v>
       </c>
       <c r="D129" t="s">
-        <v>293</v>
+        <v>18</v>
       </c>
       <c r="E129" t="s">
         <v>8</v>
       </c>
       <c r="F129" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G129" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="H129" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -7450,25 +7450,25 @@
         <v>8</v>
       </c>
       <c r="B130" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="C130" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="D130" t="s">
-        <v>295</v>
+        <v>18</v>
       </c>
       <c r="E130" t="s">
         <v>8</v>
       </c>
       <c r="F130" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G130" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
       <c r="H130" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -7476,25 +7476,25 @@
         <v>8</v>
       </c>
       <c r="B131" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="C131" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="D131" t="s">
-        <v>297</v>
+        <v>18</v>
       </c>
       <c r="E131" t="s">
         <v>8</v>
       </c>
       <c r="F131" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G131" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
       <c r="H131" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -7502,25 +7502,25 @@
         <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C132" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D132" t="s">
-        <v>299</v>
+        <v>18</v>
       </c>
       <c r="E132" t="s">
         <v>8</v>
       </c>
       <c r="F132" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G132" t="s">
-        <v>300</v>
+        <v>197</v>
       </c>
       <c r="H132" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -7528,25 +7528,25 @@
         <v>8</v>
       </c>
       <c r="B133" t="s">
-        <v>51</v>
+        <v>203</v>
       </c>
       <c r="C133" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="D133" t="s">
-        <v>302</v>
+        <v>18</v>
       </c>
       <c r="E133" t="s">
         <v>8</v>
       </c>
       <c r="F133" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="G133" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="H133" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -7554,25 +7554,25 @@
         <v>8</v>
       </c>
       <c r="B134" t="s">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="C134" t="s">
-        <v>174</v>
+        <v>17</v>
       </c>
       <c r="D134" t="s">
-        <v>304</v>
+        <v>83</v>
       </c>
       <c r="E134" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F134" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G134" t="s">
         <v>197</v>
       </c>
       <c r="H134" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -7580,19 +7580,19 @@
         <v>8</v>
       </c>
       <c r="B135" t="s">
-        <v>218</v>
+        <v>306</v>
       </c>
       <c r="C135" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D135" t="s">
-        <v>18</v>
+        <v>307</v>
       </c>
       <c r="E135" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F135" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G135" t="s">
         <v>197</v>
@@ -7615,10 +7615,10 @@
         <v>18</v>
       </c>
       <c r="E136" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F136" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G136" t="s">
         <v>197</v>
@@ -7632,19 +7632,19 @@
         <v>8</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="C137" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="D137" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="E137" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F137" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G137" t="s">
         <v>197</v>
@@ -7658,25 +7658,25 @@
         <v>8</v>
       </c>
       <c r="B138" t="s">
-        <v>34</v>
+        <v>311</v>
       </c>
       <c r="C138" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D138" t="s">
-        <v>221</v>
+        <v>312</v>
       </c>
       <c r="E138" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F138" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G138" t="s">
         <v>197</v>
       </c>
       <c r="H138" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -7684,25 +7684,25 @@
         <v>8</v>
       </c>
       <c r="B139" t="s">
-        <v>312</v>
+        <v>16</v>
       </c>
       <c r="C139" t="s">
+        <v>17</v>
+      </c>
+      <c r="D139" t="s">
+        <v>217</v>
+      </c>
+      <c r="E139" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" t="s">
         <v>313</v>
       </c>
-      <c r="D139" t="s">
-        <v>116</v>
-      </c>
-      <c r="E139" t="s">
-        <v>305</v>
-      </c>
-      <c r="F139" t="s">
-        <v>306</v>
-      </c>
       <c r="G139" t="s">
-        <v>61</v>
+        <v>197</v>
       </c>
       <c r="H139" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -7710,25 +7710,25 @@
         <v>8</v>
       </c>
       <c r="B140" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
       <c r="C140" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="D140" t="s">
-        <v>315</v>
+        <v>18</v>
       </c>
       <c r="E140" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F140" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G140" t="s">
-        <v>61</v>
+        <v>316</v>
       </c>
       <c r="H140" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -7736,22 +7736,22 @@
         <v>8</v>
       </c>
       <c r="B141" t="s">
-        <v>317</v>
+        <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="D141" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E141" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F141" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G141" t="s">
-        <v>84</v>
+        <v>316</v>
       </c>
       <c r="H141" t="s">
         <v>318</v>
@@ -7762,25 +7762,25 @@
         <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>29</v>
+        <v>173</v>
       </c>
       <c r="C142" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="D142" t="s">
-        <v>286</v>
+        <v>319</v>
       </c>
       <c r="E142" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F142" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G142" t="s">
-        <v>134</v>
+        <v>316</v>
       </c>
       <c r="H142" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -7788,25 +7788,25 @@
         <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>199</v>
+        <v>16</v>
       </c>
       <c r="C143" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D143" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="E143" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F143" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G143" t="s">
-        <v>320</v>
+        <v>14</v>
       </c>
       <c r="H143" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -7814,25 +7814,25 @@
         <v>8</v>
       </c>
       <c r="B144" t="s">
-        <v>322</v>
+        <v>29</v>
       </c>
       <c r="C144" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="D144" t="s">
         <v>323</v>
       </c>
       <c r="E144" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F144" t="s">
+        <v>313</v>
+      </c>
+      <c r="G144" t="s">
+        <v>31</v>
+      </c>
+      <c r="H144" t="s">
         <v>324</v>
-      </c>
-      <c r="G144" t="s">
-        <v>177</v>
-      </c>
-      <c r="H144" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -7840,25 +7840,25 @@
         <v>8</v>
       </c>
       <c r="B145" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C145" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D145" t="s">
+        <v>325</v>
+      </c>
+      <c r="E145" t="s">
+        <v>8</v>
+      </c>
+      <c r="F145" t="s">
+        <v>313</v>
+      </c>
+      <c r="G145" t="s">
+        <v>46</v>
+      </c>
+      <c r="H145" t="s">
         <v>326</v>
-      </c>
-      <c r="E145" t="s">
-        <v>305</v>
-      </c>
-      <c r="F145" t="s">
-        <v>324</v>
-      </c>
-      <c r="G145" t="s">
-        <v>181</v>
-      </c>
-      <c r="H145" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -7866,22 +7866,22 @@
         <v>8</v>
       </c>
       <c r="B146" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C146" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D146" t="s">
+        <v>327</v>
+      </c>
+      <c r="E146" t="s">
+        <v>8</v>
+      </c>
+      <c r="F146" t="s">
+        <v>313</v>
+      </c>
+      <c r="G146" t="s">
         <v>328</v>
-      </c>
-      <c r="E146" t="s">
-        <v>305</v>
-      </c>
-      <c r="F146" t="s">
-        <v>324</v>
-      </c>
-      <c r="G146" t="s">
-        <v>181</v>
       </c>
       <c r="H146" t="s">
         <v>329</v>
@@ -7892,22 +7892,22 @@
         <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>199</v>
+        <v>51</v>
       </c>
       <c r="C147" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D147" t="s">
-        <v>18</v>
+        <v>330</v>
       </c>
       <c r="E147" t="s">
-        <v>305</v>
+        <v>8</v>
       </c>
       <c r="F147" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="G147" t="s">
-        <v>330</v>
+        <v>183</v>
       </c>
       <c r="H147" t="s">
         <v>331</v>
@@ -7970,7 +7970,7 @@
         <v>8</v>
       </c>
       <c r="B150" t="s">
-        <v>282</v>
+        <v>311</v>
       </c>
       <c r="C150" t="s">
         <v>60</v>
@@ -8089,7 +8089,7 @@
         <v>334</v>
       </c>
       <c r="G154" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H154" t="s">
         <v>346</v>
@@ -8297,7 +8297,7 @@
         <v>352</v>
       </c>
       <c r="G162" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="H162" t="s">
         <v>359</v>
@@ -8323,7 +8323,7 @@
         <v>352</v>
       </c>
       <c r="G163" t="s">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="H163" t="s">
         <v>361</v>
@@ -8349,7 +8349,7 @@
         <v>352</v>
       </c>
       <c r="G164" t="s">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="H164" t="s">
         <v>362</v>
@@ -8490,7 +8490,7 @@
         <v>8</v>
       </c>
       <c r="B170" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C170" t="s">
         <v>35</v>
@@ -8542,7 +8542,7 @@
         <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C172" t="s">
         <v>35</v>
@@ -8574,7 +8574,7 @@
         <v>60</v>
       </c>
       <c r="D173" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="E173" t="s">
         <v>375</v>
@@ -8776,7 +8776,7 @@
         <v>8</v>
       </c>
       <c r="B181" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="C181" t="s">
         <v>35</v>
@@ -8834,7 +8834,7 @@
         <v>76</v>
       </c>
       <c r="D183" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="E183" t="s">
         <v>390</v>
@@ -8880,7 +8880,7 @@
         <v>8</v>
       </c>
       <c r="B185" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C185" t="s">
         <v>35</v>
@@ -8958,7 +8958,7 @@
         <v>8</v>
       </c>
       <c r="B188" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C188" t="s">
         <v>35</v>
@@ -9259,7 +9259,7 @@
         <v>415</v>
       </c>
       <c r="G199" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H199" t="s">
         <v>430</v>
@@ -9285,7 +9285,7 @@
         <v>415</v>
       </c>
       <c r="G200" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H200" t="s">
         <v>432</v>
@@ -9311,7 +9311,7 @@
         <v>433</v>
       </c>
       <c r="G201" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H201" t="s">
         <v>434</v>
@@ -9337,7 +9337,7 @@
         <v>433</v>
       </c>
       <c r="G202" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H202" t="s">
         <v>436</v>
@@ -9363,7 +9363,7 @@
         <v>433</v>
       </c>
       <c r="G203" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H203" t="s">
         <v>438</v>
@@ -9389,7 +9389,7 @@
         <v>433</v>
       </c>
       <c r="G204" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H204" t="s">
         <v>440</v>
@@ -9415,7 +9415,7 @@
         <v>433</v>
       </c>
       <c r="G205" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H205" t="s">
         <v>442</v>
@@ -10076,7 +10076,7 @@
         <v>8</v>
       </c>
       <c r="B231" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="C231" t="s">
         <v>30</v>
@@ -10299,7 +10299,7 @@
         <v>491</v>
       </c>
       <c r="G239" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H239" t="s">
         <v>504</v>
@@ -10325,7 +10325,7 @@
         <v>491</v>
       </c>
       <c r="G240" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H240" t="s">
         <v>506</v>
@@ -10599,7 +10599,7 @@
         <v>527</v>
       </c>
       <c r="C251" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D251" t="s">
         <v>18</v>
@@ -10654,7 +10654,7 @@
         <v>35</v>
       </c>
       <c r="D253" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="E253" t="s">
         <v>414</v>
@@ -10706,7 +10706,7 @@
         <v>30</v>
       </c>
       <c r="D255" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="E255" t="s">
         <v>414</v>
@@ -10729,7 +10729,7 @@
         <v>527</v>
       </c>
       <c r="C256" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D256" t="s">
         <v>18</v>
@@ -10781,7 +10781,7 @@
         <v>527</v>
       </c>
       <c r="C258" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D258" t="s">
         <v>18</v>
@@ -11012,10 +11012,10 @@
         <v>8</v>
       </c>
       <c r="B267" t="s">
-        <v>312</v>
+        <v>209</v>
       </c>
       <c r="C267" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D267" t="s">
         <v>18</v>
@@ -11079,7 +11079,7 @@
         <v>550</v>
       </c>
       <c r="G269" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H269" t="s">
         <v>559</v>
@@ -11105,7 +11105,7 @@
         <v>550</v>
       </c>
       <c r="G270" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H270" t="s">
         <v>560</v>
@@ -11131,7 +11131,7 @@
         <v>550</v>
       </c>
       <c r="G271" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="H271" t="s">
         <v>563</v>
@@ -11157,7 +11157,7 @@
         <v>550</v>
       </c>
       <c r="G272" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="H272" t="s">
         <v>564</v>
@@ -11183,7 +11183,7 @@
         <v>550</v>
       </c>
       <c r="G273" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="H273" t="s">
         <v>565</v>
@@ -11486,7 +11486,7 @@
         <v>30</v>
       </c>
       <c r="D285" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="E285" t="s">
         <v>583</v>
@@ -11662,7 +11662,7 @@
         <v>8</v>
       </c>
       <c r="B292" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C292" t="s">
         <v>35</v>
@@ -11714,7 +11714,7 @@
         <v>8</v>
       </c>
       <c r="B294" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C294" t="s">
         <v>35</v>
@@ -11740,7 +11740,7 @@
         <v>8</v>
       </c>
       <c r="B295" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C295" t="s">
         <v>35</v>
@@ -11922,7 +11922,7 @@
         <v>8</v>
       </c>
       <c r="B302" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C302" t="s">
         <v>35</v>
@@ -12052,7 +12052,7 @@
         <v>8</v>
       </c>
       <c r="B307" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C307" t="s">
         <v>35</v>
@@ -12130,7 +12130,7 @@
         <v>8</v>
       </c>
       <c r="B310" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C310" t="s">
         <v>35</v>
@@ -12208,7 +12208,7 @@
         <v>8</v>
       </c>
       <c r="B313" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C313" t="s">
         <v>35</v>
@@ -12223,7 +12223,7 @@
         <v>653</v>
       </c>
       <c r="G313" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
       <c r="H313" t="s">
         <v>654</v>
@@ -12575,7 +12575,7 @@
         <v>687</v>
       </c>
       <c r="C327" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D327" t="s">
         <v>18</v>
@@ -12627,7 +12627,7 @@
         <v>687</v>
       </c>
       <c r="C329" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D329" t="s">
         <v>18</v>
@@ -12780,13 +12780,13 @@
         <v>8</v>
       </c>
       <c r="B335" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C335" t="s">
         <v>35</v>
       </c>
       <c r="D335" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="E335" t="s">
         <v>702</v>
@@ -12977,7 +12977,7 @@
         <v>707</v>
       </c>
       <c r="G342" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H342" t="s">
         <v>716</v>
@@ -13003,7 +13003,7 @@
         <v>707</v>
       </c>
       <c r="G343" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H343" t="s">
         <v>717</v>
@@ -13121,7 +13121,7 @@
         <v>687</v>
       </c>
       <c r="C348" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D348" t="s">
         <v>18</v>
@@ -13263,7 +13263,7 @@
         <v>738</v>
       </c>
       <c r="G353" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H353" t="s">
         <v>739</v>
@@ -13326,7 +13326,7 @@
         <v>8</v>
       </c>
       <c r="B356" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="C356" t="s">
         <v>30</v>
@@ -13378,7 +13378,7 @@
         <v>8</v>
       </c>
       <c r="B358" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C358" t="s">
         <v>100</v>
@@ -13430,7 +13430,7 @@
         <v>8</v>
       </c>
       <c r="B360" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C360" t="s">
         <v>100</v>
@@ -13508,7 +13508,7 @@
         <v>8</v>
       </c>
       <c r="B363" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="C363" t="s">
         <v>35</v>
@@ -13534,7 +13534,7 @@
         <v>8</v>
       </c>
       <c r="B364" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C364" t="s">
         <v>100</v>
@@ -13586,7 +13586,7 @@
         <v>8</v>
       </c>
       <c r="B366" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="C366" t="s">
         <v>35</v>
@@ -13679,7 +13679,7 @@
         <v>774</v>
       </c>
       <c r="G369" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H369" t="s">
         <v>775</v>
@@ -13705,7 +13705,7 @@
         <v>774</v>
       </c>
       <c r="G370" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H370" t="s">
         <v>777</v>
@@ -13774,7 +13774,7 @@
         <v>87</v>
       </c>
       <c r="D373" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="E373" t="s">
         <v>773</v>
@@ -14028,7 +14028,7 @@
         <v>8</v>
       </c>
       <c r="B383" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C383" t="s">
         <v>35</v>
@@ -14069,7 +14069,7 @@
         <v>800</v>
       </c>
       <c r="G384" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="H384" t="s">
         <v>803</v>
@@ -14121,7 +14121,7 @@
         <v>800</v>
       </c>
       <c r="G386" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="H386" t="s">
         <v>803</v>
@@ -14184,10 +14184,10 @@
         <v>8</v>
       </c>
       <c r="B389" t="s">
-        <v>312</v>
+        <v>209</v>
       </c>
       <c r="C389" t="s">
-        <v>313</v>
+        <v>210</v>
       </c>
       <c r="D389" t="s">
         <v>116</v>
@@ -14251,7 +14251,7 @@
         <v>815</v>
       </c>
       <c r="G391" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H391" t="s">
         <v>816</v>
@@ -14502,7 +14502,7 @@
         <v>17</v>
       </c>
       <c r="D401" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="E401" t="s">
         <v>832</v>
@@ -14522,7 +14522,7 @@
         <v>8</v>
       </c>
       <c r="B402" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C402" t="s">
         <v>100</v>
@@ -14537,7 +14537,7 @@
         <v>837</v>
       </c>
       <c r="G402" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H402" t="s">
         <v>838</v>
@@ -14589,7 +14589,7 @@
         <v>837</v>
       </c>
       <c r="G404" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H404" t="s">
         <v>840</v>
@@ -14641,7 +14641,7 @@
         <v>842</v>
       </c>
       <c r="G406" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H406" t="s">
         <v>843</v>
@@ -14797,7 +14797,7 @@
         <v>845</v>
       </c>
       <c r="G412" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H412" t="s">
         <v>851</v>
@@ -14927,7 +14927,7 @@
         <v>853</v>
       </c>
       <c r="G417" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="H417" t="s">
         <v>858</v>

</xml_diff>